<commit_message>
Add 710 to electives list
</commit_message>
<xml_diff>
--- a/docs/PhD-electives-list.xlsx
+++ b/docs/PhD-electives-list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samharper/git/epi-phd/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{048AE5D0-1F06-5441-B7C9-61583844135A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A106A72B-D61E-B745-B2C6-8734B2A3A6F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="460" windowWidth="28080" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="460" windowWidth="28080" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="55">
   <si>
     <t>Course</t>
   </si>
@@ -181,7 +181,10 @@
     <t>PPHS 684 Special Topics: Foundations of Health Promotion</t>
   </si>
   <si>
-    <t>Last edited: 2021-05-27 by Sam Harper</t>
+    <t>EPIB 710 Advanced Causal Inference</t>
+  </si>
+  <si>
+    <t>Last edited: 2022-06-07 by Sam Harper</t>
   </si>
 </sst>
 </file>
@@ -516,9 +519,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -544,7 +549,7 @@
       </c>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -555,7 +560,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -566,7 +571,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" ht="15">
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
@@ -577,7 +582,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="15">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -588,7 +593,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="15">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -599,7 +604,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="15">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -610,7 +615,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" ht="15">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -621,7 +626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="15">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -632,7 +637,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="15">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
@@ -643,7 +648,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="15">
       <c r="A11" s="7" t="s">
         <v>15</v>
       </c>
@@ -654,7 +659,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="15">
       <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
@@ -665,7 +670,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="15">
       <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
@@ -676,7 +681,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="15">
       <c r="A14" s="3" t="s">
         <v>18</v>
       </c>
@@ -687,7 +692,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" ht="15">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
@@ -699,7 +704,7 @@
       </c>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" ht="15">
       <c r="A16" s="7" t="s">
         <v>20</v>
       </c>
@@ -711,7 +716,7 @@
       </c>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" ht="15">
       <c r="A17" s="7" t="s">
         <v>21</v>
       </c>
@@ -725,7 +730,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" ht="15">
       <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
@@ -736,7 +741,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" ht="15">
       <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
@@ -747,7 +752,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" ht="15">
       <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
@@ -758,7 +763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" ht="15">
       <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
@@ -769,7 +774,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" ht="15">
       <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
@@ -780,7 +785,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" ht="15">
       <c r="A23" s="7" t="s">
         <v>28</v>
       </c>
@@ -791,7 +796,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" ht="15">
       <c r="A24" s="10" t="s">
         <v>29</v>
       </c>
@@ -802,7 +807,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" ht="15">
       <c r="A25" s="7" t="s">
         <v>30</v>
       </c>
@@ -813,7 +818,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" ht="15">
       <c r="A26" s="3" t="s">
         <v>31</v>
       </c>
@@ -824,7 +829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" ht="15">
       <c r="A27" s="3" t="s">
         <v>32</v>
       </c>
@@ -835,7 +840,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" ht="15">
       <c r="A28" s="3" t="s">
         <v>33</v>
       </c>
@@ -846,7 +851,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" ht="15">
       <c r="A29" s="3" t="s">
         <v>34</v>
       </c>
@@ -857,199 +862,210 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:4" ht="15">
+      <c r="A30" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="4">
+        <v>3</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15">
+      <c r="A31" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="4">
-        <v>3</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="3" t="s">
+      <c r="B31" s="4">
+        <v>3</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15">
+      <c r="A32" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="4">
-        <v>3</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="3" t="s">
+      <c r="B32" s="4">
+        <v>3</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15">
+      <c r="A33" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="4">
-        <v>3</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="3" t="s">
+      <c r="B33" s="4">
+        <v>3</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15">
+      <c r="A34" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="4">
-        <v>3</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="3" t="s">
+      <c r="B34" s="4">
+        <v>3</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15">
+      <c r="A35" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="4">
-        <v>3</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="3" t="s">
+      <c r="B35" s="4">
+        <v>3</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15">
+      <c r="A36" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="4">
-        <v>3</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="3" t="s">
+      <c r="B36" s="4">
+        <v>3</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15">
+      <c r="A37" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="4">
-        <v>3</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="3" t="s">
+      <c r="B37" s="4">
+        <v>3</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15">
+      <c r="A38" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="4">
-        <v>3</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="3" t="s">
+      <c r="B38" s="4">
+        <v>3</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15">
+      <c r="A39" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="4">
-        <v>3</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="3" t="s">
+      <c r="B39" s="4">
+        <v>3</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15">
+      <c r="A40" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="4">
-        <v>3</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="7" t="s">
+      <c r="B40" s="4">
+        <v>3</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15">
+      <c r="A41" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="4">
-        <v>3</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="7" t="s">
+      <c r="B41" s="4">
+        <v>3</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15">
+      <c r="A42" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="4">
-        <v>3</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="3" t="s">
+      <c r="B42" s="4">
+        <v>3</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15">
+      <c r="A43" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="4">
-        <v>3</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="3" t="s">
+      <c r="B43" s="4">
+        <v>3</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15">
+      <c r="A44" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="4">
-        <v>3</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="11" t="s">
+      <c r="B44" s="4">
+        <v>3</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15">
+      <c r="A45" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="4">
+      <c r="B45" s="4">
         <v>2</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D44" s="4" t="s">
+      <c r="C45" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A45" s="12" t="s">
+    <row r="46" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A46" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="4">
-        <v>3</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="10" t="s">
+      <c r="B46" s="4">
+        <v>3</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15">
+      <c r="A47" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="4">
-        <v>3</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A47" s="13" t="s">
-        <v>53</v>
+      <c r="B47" s="4">
+        <v>3</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A48" s="13" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>